<commit_message>
Datasets to english and criteriaevalchain
</commit_message>
<xml_diff>
--- a/resources/datasets/qaevalchain/dataset.xlsx
+++ b/resources/datasets/qaevalchain/dataset.xlsx
@@ -22,16 +22,16 @@
     <t>answer</t>
   </si>
   <si>
-    <t>¿Cuál es la capital de Francia?</t>
-  </si>
-  <si>
-    <t>¿Quién escribió Cien años de soledad?</t>
-  </si>
-  <si>
-    <t>¿En qué año llegó el hombre a la Luna?</t>
-  </si>
-  <si>
-    <t>París</t>
+    <t>What is the capital of France?</t>
+  </si>
+  <si>
+    <t>Who wrote One Hundred Years of Solitude?</t>
+  </si>
+  <si>
+    <t>What year did man land on the Moon?</t>
+  </si>
+  <si>
+    <t>Paris</t>
   </si>
   <si>
     <t>Gabriel García Márquez</t>

</xml_diff>